<commit_message>
Update stelah bimbingan revisi
</commit_message>
<xml_diff>
--- a/Latihan/output/bobot_bilstm.xlsx
+++ b/Latihan/output/bobot_bilstm.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,19 +443,31 @@
       <c r="D1" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.09226408453054369</v>
+        <v>-0.01014579726076258</v>
       </c>
       <c r="C2" t="n">
-        <v>0.09773935644102011</v>
+        <v>0.02666081550071997</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.1149013322465454</v>
+        <v>-0.0767144750377244</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-0.03678720286518841</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.08551102827500009</v>
       </c>
     </row>
     <row r="3">
@@ -463,13 +475,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.05543787997817162</v>
+        <v>0.002350303899347969</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.09028449794670225</v>
+        <v>0.05708249221189834</v>
       </c>
       <c r="D3" t="n">
-        <v>0.08763403916897244</v>
+        <v>0.1002612127618704</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-0.06442888459132723</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-0.09187687035283353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>